<commit_message>
Print Leads - Error For Jalani
</commit_message>
<xml_diff>
--- a/UDM.Insurance.Interface/Templates/PrintTemplateSheMaccBase.xlsx
+++ b/UDM.Insurance.Interface/Templates/PrintTemplateSheMaccBase.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TyronR\Desktop\Source\udminsure\UDM.Insurance.Interface\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DaneB\source\repos\Insure\UDM.Insurance.Interface\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D94912E-E37A-43D9-9241-6534F232ACC1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C26E026-3A86-4CA5-9353-6AE5772168FA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="4" r:id="rId1"/>
@@ -761,6 +761,99 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -776,98 +869,221 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -875,51 +1091,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -949,177 +1120,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1593,21 +1593,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:F22"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageLayout" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.265625" customWidth="1"/>
-    <col min="2" max="3" width="24.73046875" customWidth="1"/>
-    <col min="4" max="4" width="12.73046875" customWidth="1"/>
-    <col min="5" max="5" width="24.73046875" customWidth="1"/>
-    <col min="6" max="6" width="12.73046875" customWidth="1"/>
-    <col min="7" max="7" width="19.265625" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="2" max="3" width="24.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" customWidth="1"/>
+    <col min="7" max="7" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="24" t="s">
         <v>17</v>
       </c>
@@ -1616,7 +1616,7 @@
       <c r="E2" s="24"/>
       <c r="F2" s="24"/>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
@@ -1633,126 +1633,126 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -1773,156 +1773,156 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:O29"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8:H8"/>
+    <sheetView view="pageLayout" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6:H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" ht="25.5" x14ac:dyDescent="0.75">
-      <c r="B2" s="49" t="s">
+    <row r="2" spans="2:14" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="B2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="50"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="54"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="30"/>
       <c r="K2" s="6"/>
     </row>
-    <row r="3" spans="2:14" ht="21" x14ac:dyDescent="0.65">
-      <c r="B3" s="55" t="s">
+    <row r="3" spans="2:14" ht="21" x14ac:dyDescent="0.35">
+      <c r="B3" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="56"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="58"/>
-      <c r="F3" s="59"/>
-      <c r="G3" s="59"/>
-      <c r="H3" s="60"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="36"/>
       <c r="K3" s="7"/>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="G4" s="5"/>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B6" s="34" t="s">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B6" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="35"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="48"/>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B7" s="34" t="s">
+      <c r="C6" s="38"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="42"/>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B7" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="35"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="47"/>
-      <c r="G7" s="47"/>
-      <c r="H7" s="48"/>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B8" s="34" t="s">
+      <c r="C7" s="38"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="41"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="42"/>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B8" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="35"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="47"/>
-      <c r="G8" s="47"/>
-      <c r="H8" s="48"/>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B9" s="34" t="s">
+      <c r="C8" s="38"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="42"/>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B9" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="35"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="47"/>
-      <c r="G9" s="47"/>
-      <c r="H9" s="48"/>
-    </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B10" s="34" t="s">
+      <c r="C9" s="38"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="42"/>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B10" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="35"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="39"/>
-    </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B13" s="34" t="s">
+      <c r="C10" s="38"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="45"/>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B13" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="35"/>
-      <c r="D13" s="36"/>
-      <c r="E13" s="34" t="s">
+      <c r="C13" s="38"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="35"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="36"/>
-    </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B14" s="40"/>
-      <c r="C14" s="41"/>
-      <c r="D14" s="42"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="44"/>
-      <c r="G14" s="44"/>
-      <c r="H14" s="45"/>
-    </row>
-    <row r="16" spans="2:14" ht="23.25" x14ac:dyDescent="0.7">
-      <c r="B16" s="30" t="s">
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="39"/>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B14" s="46"/>
+      <c r="C14" s="47"/>
+      <c r="D14" s="48"/>
+      <c r="E14" s="49"/>
+      <c r="F14" s="50"/>
+      <c r="G14" s="50"/>
+      <c r="H14" s="51"/>
+    </row>
+    <row r="16" spans="2:14" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B16" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="30"/>
+      <c r="C16" s="52"/>
+      <c r="D16" s="52"/>
+      <c r="E16" s="52"/>
+      <c r="F16" s="52"/>
       <c r="G16" s="20"/>
       <c r="H16" s="20"/>
-      <c r="I16" s="30" t="s">
+      <c r="I16" s="52" t="s">
         <v>46</v>
       </c>
-      <c r="J16" s="30"/>
-      <c r="K16" s="30"/>
-      <c r="L16" s="30"/>
-      <c r="M16" s="30"/>
+      <c r="J16" s="52"/>
+      <c r="K16" s="52"/>
+      <c r="L16" s="52"/>
+      <c r="M16" s="52"/>
       <c r="N16" s="8"/>
     </row>
-    <row r="17" spans="2:15" ht="22.9" x14ac:dyDescent="0.65">
-      <c r="B17" s="31" t="s">
+    <row r="17" spans="2:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B17" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="32"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="33"/>
+      <c r="C17" s="54"/>
+      <c r="D17" s="54"/>
+      <c r="E17" s="54"/>
+      <c r="F17" s="55"/>
       <c r="G17" s="21"/>
-      <c r="I17" s="31" t="s">
+      <c r="I17" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="J17" s="32"/>
-      <c r="K17" s="32"/>
-      <c r="L17" s="32"/>
-      <c r="M17" s="33"/>
-    </row>
-    <row r="18" spans="2:15" ht="22.9" x14ac:dyDescent="0.65">
+      <c r="J17" s="54"/>
+      <c r="K17" s="54"/>
+      <c r="L17" s="54"/>
+      <c r="M17" s="55"/>
+    </row>
+    <row r="18" spans="2:15" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B18" s="22"/>
       <c r="C18" s="22"/>
       <c r="D18" s="22"/>
@@ -1934,7 +1934,7 @@
       <c r="L18" s="22"/>
       <c r="M18" s="22"/>
     </row>
-    <row r="19" spans="2:15" ht="22.9" x14ac:dyDescent="0.65">
+    <row r="19" spans="2:15" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B19" s="22"/>
       <c r="C19" s="22"/>
       <c r="D19" s="22"/>
@@ -1946,7 +1946,7 @@
       <c r="L19" s="22"/>
       <c r="M19" s="22"/>
     </row>
-    <row r="20" spans="2:15" ht="22.9" x14ac:dyDescent="0.65">
+    <row r="20" spans="2:15" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B20" s="22"/>
       <c r="C20" s="22"/>
       <c r="D20" s="22"/>
@@ -1958,7 +1958,7 @@
       <c r="L20" s="22"/>
       <c r="M20" s="22"/>
     </row>
-    <row r="21" spans="2:15" ht="22.9" x14ac:dyDescent="0.65">
+    <row r="21" spans="2:15" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B21" s="22"/>
       <c r="C21" s="22"/>
       <c r="D21" s="22"/>
@@ -1970,7 +1970,7 @@
       <c r="L21" s="22"/>
       <c r="M21" s="22"/>
     </row>
-    <row r="22" spans="2:15" ht="22.9" x14ac:dyDescent="0.65">
+    <row r="22" spans="2:15" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B22" s="22"/>
       <c r="C22" s="22"/>
       <c r="D22" s="22"/>
@@ -1982,51 +1982,51 @@
       <c r="L22" s="22"/>
       <c r="M22" s="22"/>
     </row>
-    <row r="23" spans="2:15" ht="22.9" x14ac:dyDescent="0.65">
-      <c r="I23" s="31" t="s">
+    <row r="23" spans="2:15" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="I23" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="J23" s="32"/>
-      <c r="K23" s="32"/>
-      <c r="L23" s="32"/>
-      <c r="M23" s="33"/>
-    </row>
-    <row r="24" spans="2:15" ht="22.9" x14ac:dyDescent="0.65">
+      <c r="J23" s="54"/>
+      <c r="K23" s="54"/>
+      <c r="L23" s="54"/>
+      <c r="M23" s="55"/>
+    </row>
+    <row r="24" spans="2:15" ht="23.25" x14ac:dyDescent="0.35">
       <c r="I24" s="23"/>
       <c r="J24" s="23"/>
       <c r="K24" s="23"/>
       <c r="L24" s="23"/>
       <c r="M24" s="23"/>
     </row>
-    <row r="26" spans="2:15" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="B26" s="27" t="s">
+    <row r="26" spans="2:15" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B26" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="C26" s="28"/>
-      <c r="D26" s="29"/>
-      <c r="E26" s="25" t="s">
+      <c r="C26" s="59"/>
+      <c r="D26" s="60"/>
+      <c r="E26" s="56" t="s">
         <v>49</v>
       </c>
-      <c r="F26" s="26"/>
-      <c r="G26" s="25" t="s">
+      <c r="F26" s="57"/>
+      <c r="G26" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="H26" s="26"/>
-      <c r="I26" s="25" t="s">
+      <c r="H26" s="57"/>
+      <c r="I26" s="56" t="s">
         <v>25</v>
       </c>
-      <c r="J26" s="26"/>
-      <c r="K26" s="25" t="s">
+      <c r="J26" s="57"/>
+      <c r="K26" s="56" t="s">
         <v>51</v>
       </c>
-      <c r="L26" s="26"/>
-      <c r="M26" s="25" t="s">
+      <c r="L26" s="57"/>
+      <c r="M26" s="56" t="s">
         <v>52</v>
       </c>
-      <c r="N26" s="26"/>
+      <c r="N26" s="57"/>
       <c r="O26"/>
     </row>
-    <row r="27" spans="2:15" s="8" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:15" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27"/>
       <c r="C27"/>
       <c r="D27"/>
@@ -2042,7 +2042,7 @@
       <c r="N27"/>
       <c r="O27"/>
     </row>
-    <row r="28" spans="2:15" s="8" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:15" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28"/>
       <c r="C28"/>
       <c r="D28"/>
@@ -2058,7 +2058,7 @@
       <c r="N28"/>
       <c r="O28"/>
     </row>
-    <row r="29" spans="2:15" s="8" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:15" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29"/>
       <c r="C29"/>
       <c r="D29"/>
@@ -2076,35 +2076,35 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="I16:M16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="I17:M17"/>
+    <mergeCell ref="I23:M23"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="E10:H10"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="E13:H13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="E14:H14"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="E7:H7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="E8:H8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="E9:H9"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="E2:H2"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="E3:H3"/>
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="E6:H6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="E7:H7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="E8:H8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="E9:H9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="E10:H10"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="E13:H13"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="E14:H14"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="I16:M16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="I17:M17"/>
-    <mergeCell ref="I23:M23"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="K26:L26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -2118,17 +2118,17 @@
   </sheetPr>
   <dimension ref="A1:BT45"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A25" zoomScale="130" zoomScaleNormal="100" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="AG26" sqref="AG26:BA26"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="130" zoomScaleNormal="100" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="BJ40" sqref="BJ40:BK42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="10.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="122" width="2" style="3" customWidth="1"/>
-    <col min="123" max="16384" width="9.1328125" style="3"/>
+    <col min="123" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:70" x14ac:dyDescent="0.35">
+    <row r="1" spans="3:70" x14ac:dyDescent="0.2">
       <c r="C1" s="11"/>
       <c r="D1" s="12"/>
       <c r="E1" s="19"/>
@@ -2198,7 +2198,7 @@
       <c r="BQ1" s="10"/>
       <c r="BR1" s="11"/>
     </row>
-    <row r="2" spans="3:70" x14ac:dyDescent="0.35">
+    <row r="2" spans="3:70" x14ac:dyDescent="0.2">
       <c r="C2" s="11"/>
       <c r="D2" s="12"/>
       <c r="E2" s="11"/>
@@ -2268,7 +2268,7 @@
       <c r="BQ2" s="10"/>
       <c r="BR2" s="11"/>
     </row>
-    <row r="3" spans="3:70" x14ac:dyDescent="0.35">
+    <row r="3" spans="3:70" x14ac:dyDescent="0.2">
       <c r="C3" s="11"/>
       <c r="D3" s="12"/>
       <c r="E3" s="11"/>
@@ -2338,7 +2338,7 @@
       <c r="BQ3" s="10"/>
       <c r="BR3" s="11"/>
     </row>
-    <row r="4" spans="3:70" x14ac:dyDescent="0.35">
+    <row r="4" spans="3:70" x14ac:dyDescent="0.2">
       <c r="C4" s="11"/>
       <c r="D4" s="12"/>
       <c r="E4" s="11"/>
@@ -2408,7 +2408,7 @@
       <c r="BQ4" s="10"/>
       <c r="BR4" s="11"/>
     </row>
-    <row r="5" spans="3:70" x14ac:dyDescent="0.35">
+    <row r="5" spans="3:70" x14ac:dyDescent="0.2">
       <c r="C5" s="11"/>
       <c r="D5" s="12"/>
       <c r="E5" s="11"/>
@@ -2478,7 +2478,7 @@
       <c r="BQ5" s="10"/>
       <c r="BR5" s="11"/>
     </row>
-    <row r="6" spans="3:70" x14ac:dyDescent="0.35">
+    <row r="6" spans="3:70" x14ac:dyDescent="0.2">
       <c r="C6" s="11"/>
       <c r="D6" s="12"/>
       <c r="E6" s="11"/>
@@ -2548,7 +2548,7 @@
       <c r="BQ6" s="10"/>
       <c r="BR6" s="11"/>
     </row>
-    <row r="7" spans="3:70" x14ac:dyDescent="0.35">
+    <row r="7" spans="3:70" x14ac:dyDescent="0.2">
       <c r="C7" s="11"/>
       <c r="D7" s="12"/>
       <c r="E7" s="11"/>
@@ -2618,7 +2618,7 @@
       <c r="BQ7" s="10"/>
       <c r="BR7" s="11"/>
     </row>
-    <row r="8" spans="3:70" x14ac:dyDescent="0.35">
+    <row r="8" spans="3:70" x14ac:dyDescent="0.2">
       <c r="C8" s="11"/>
       <c r="D8" s="12"/>
       <c r="E8" s="11"/>
@@ -2688,7 +2688,7 @@
       <c r="BQ8" s="10"/>
       <c r="BR8" s="11"/>
     </row>
-    <row r="9" spans="3:70" x14ac:dyDescent="0.35">
+    <row r="9" spans="3:70" x14ac:dyDescent="0.2">
       <c r="C9" s="11"/>
       <c r="D9" s="12"/>
       <c r="E9" s="11"/>
@@ -2758,7 +2758,7 @@
       <c r="BQ9" s="10"/>
       <c r="BR9" s="11"/>
     </row>
-    <row r="10" spans="3:70" x14ac:dyDescent="0.35">
+    <row r="10" spans="3:70" x14ac:dyDescent="0.2">
       <c r="C10" s="11"/>
       <c r="D10" s="12"/>
       <c r="E10" s="11"/>
@@ -2828,7 +2828,7 @@
       <c r="BQ10" s="10"/>
       <c r="BR10" s="11"/>
     </row>
-    <row r="11" spans="3:70" x14ac:dyDescent="0.35">
+    <row r="11" spans="3:70" x14ac:dyDescent="0.2">
       <c r="C11" s="11"/>
       <c r="D11" s="12"/>
       <c r="E11" s="11"/>
@@ -2898,7 +2898,7 @@
       <c r="BQ11" s="10"/>
       <c r="BR11" s="11"/>
     </row>
-    <row r="12" spans="3:70" x14ac:dyDescent="0.35">
+    <row r="12" spans="3:70" x14ac:dyDescent="0.2">
       <c r="C12" s="11"/>
       <c r="D12" s="12"/>
       <c r="E12" s="11"/>
@@ -2968,7 +2968,7 @@
       <c r="BQ12" s="10"/>
       <c r="BR12" s="11"/>
     </row>
-    <row r="13" spans="3:70" x14ac:dyDescent="0.35">
+    <row r="13" spans="3:70" x14ac:dyDescent="0.2">
       <c r="C13" s="11"/>
       <c r="D13" s="12"/>
       <c r="E13" s="11"/>
@@ -3038,7 +3038,7 @@
       <c r="BQ13" s="10"/>
       <c r="BR13" s="11"/>
     </row>
-    <row r="14" spans="3:70" x14ac:dyDescent="0.35">
+    <row r="14" spans="3:70" x14ac:dyDescent="0.2">
       <c r="C14" s="11"/>
       <c r="D14" s="12"/>
       <c r="E14" s="11"/>
@@ -3108,7 +3108,7 @@
       <c r="BQ14" s="10"/>
       <c r="BR14" s="11"/>
     </row>
-    <row r="15" spans="3:70" x14ac:dyDescent="0.35">
+    <row r="15" spans="3:70" x14ac:dyDescent="0.2">
       <c r="C15" s="11"/>
       <c r="D15" s="12"/>
       <c r="E15" s="11"/>
@@ -3178,7 +3178,7 @@
       <c r="BQ15" s="10"/>
       <c r="BR15" s="11"/>
     </row>
-    <row r="16" spans="3:70" x14ac:dyDescent="0.35">
+    <row r="16" spans="3:70" x14ac:dyDescent="0.2">
       <c r="C16" s="11"/>
       <c r="D16" s="12"/>
       <c r="E16" s="11"/>
@@ -3248,7 +3248,7 @@
       <c r="BQ16" s="10"/>
       <c r="BR16" s="11"/>
     </row>
-    <row r="17" spans="3:70" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:70" x14ac:dyDescent="0.2">
       <c r="C17" s="11"/>
       <c r="D17" s="12"/>
       <c r="E17" s="11"/>
@@ -3318,7 +3318,7 @@
       <c r="BQ17" s="10"/>
       <c r="BR17" s="11"/>
     </row>
-    <row r="18" spans="3:70" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:70" x14ac:dyDescent="0.2">
       <c r="C18" s="11"/>
       <c r="D18" s="12"/>
       <c r="E18" s="11"/>
@@ -3388,7 +3388,7 @@
       <c r="BQ18" s="10"/>
       <c r="BR18" s="11"/>
     </row>
-    <row r="19" spans="3:70" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:70" x14ac:dyDescent="0.2">
       <c r="C19" s="11"/>
       <c r="D19" s="12"/>
       <c r="E19" s="11"/>
@@ -3458,7 +3458,7 @@
       <c r="BQ19" s="10"/>
       <c r="BR19" s="11"/>
     </row>
-    <row r="20" spans="3:70" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:70" x14ac:dyDescent="0.2">
       <c r="C20" s="11"/>
       <c r="D20" s="12"/>
       <c r="E20" s="11"/>
@@ -3528,7 +3528,7 @@
       <c r="BQ20" s="10"/>
       <c r="BR20" s="11"/>
     </row>
-    <row r="21" spans="3:70" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:70" x14ac:dyDescent="0.2">
       <c r="C21" s="11"/>
       <c r="D21" s="12"/>
       <c r="E21" s="11"/>
@@ -3598,7 +3598,7 @@
       <c r="BQ21" s="10"/>
       <c r="BR21" s="11"/>
     </row>
-    <row r="22" spans="3:70" ht="10.9" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="3:70" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C22" s="11"/>
       <c r="D22" s="12"/>
       <c r="E22" s="11"/>
@@ -3668,7 +3668,7 @@
       <c r="BQ22" s="10"/>
       <c r="BR22" s="11"/>
     </row>
-    <row r="23" spans="3:70" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.65">
+    <row r="23" spans="3:70" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="C23" s="15"/>
       <c r="D23" s="17"/>
       <c r="E23" s="15"/>
@@ -3687,41 +3687,41 @@
       <c r="R23" s="15"/>
       <c r="S23" s="15"/>
       <c r="T23" s="15"/>
-      <c r="U23" s="121" t="s">
+      <c r="U23" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="V23" s="122"/>
-      <c r="W23" s="122"/>
-      <c r="X23" s="122"/>
-      <c r="Y23" s="122"/>
-      <c r="Z23" s="122"/>
-      <c r="AA23" s="122"/>
-      <c r="AB23" s="122"/>
-      <c r="AC23" s="122"/>
-      <c r="AD23" s="122"/>
-      <c r="AE23" s="122"/>
-      <c r="AF23" s="122"/>
-      <c r="AG23" s="123"/>
-      <c r="AH23" s="123"/>
-      <c r="AI23" s="123"/>
-      <c r="AJ23" s="123"/>
-      <c r="AK23" s="123"/>
-      <c r="AL23" s="123"/>
-      <c r="AM23" s="123"/>
-      <c r="AN23" s="123"/>
-      <c r="AO23" s="123"/>
-      <c r="AP23" s="123"/>
-      <c r="AQ23" s="123"/>
-      <c r="AR23" s="123"/>
-      <c r="AS23" s="123"/>
-      <c r="AT23" s="123"/>
-      <c r="AU23" s="123"/>
-      <c r="AV23" s="123"/>
-      <c r="AW23" s="123"/>
-      <c r="AX23" s="123"/>
-      <c r="AY23" s="123"/>
-      <c r="AZ23" s="123"/>
-      <c r="BA23" s="124"/>
+      <c r="V23" s="79"/>
+      <c r="W23" s="79"/>
+      <c r="X23" s="79"/>
+      <c r="Y23" s="79"/>
+      <c r="Z23" s="79"/>
+      <c r="AA23" s="79"/>
+      <c r="AB23" s="79"/>
+      <c r="AC23" s="79"/>
+      <c r="AD23" s="79"/>
+      <c r="AE23" s="79"/>
+      <c r="AF23" s="79"/>
+      <c r="AG23" s="80"/>
+      <c r="AH23" s="80"/>
+      <c r="AI23" s="80"/>
+      <c r="AJ23" s="80"/>
+      <c r="AK23" s="80"/>
+      <c r="AL23" s="80"/>
+      <c r="AM23" s="80"/>
+      <c r="AN23" s="80"/>
+      <c r="AO23" s="80"/>
+      <c r="AP23" s="80"/>
+      <c r="AQ23" s="80"/>
+      <c r="AR23" s="80"/>
+      <c r="AS23" s="80"/>
+      <c r="AT23" s="80"/>
+      <c r="AU23" s="80"/>
+      <c r="AV23" s="80"/>
+      <c r="AW23" s="80"/>
+      <c r="AX23" s="80"/>
+      <c r="AY23" s="80"/>
+      <c r="AZ23" s="80"/>
+      <c r="BA23" s="81"/>
       <c r="BB23" s="15"/>
       <c r="BC23" s="15"/>
       <c r="BD23" s="15"/>
@@ -3740,7 +3740,7 @@
       <c r="BQ23" s="14"/>
       <c r="BR23" s="15"/>
     </row>
-    <row r="24" spans="3:70" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.65">
+    <row r="24" spans="3:70" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="C24" s="15"/>
       <c r="D24" s="17"/>
       <c r="E24" s="15"/>
@@ -3759,41 +3759,41 @@
       <c r="R24" s="15"/>
       <c r="S24" s="15"/>
       <c r="T24" s="15"/>
-      <c r="U24" s="119" t="s">
+      <c r="U24" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="V24" s="120"/>
-      <c r="W24" s="120"/>
-      <c r="X24" s="120"/>
-      <c r="Y24" s="120"/>
-      <c r="Z24" s="120"/>
-      <c r="AA24" s="120"/>
-      <c r="AB24" s="120"/>
-      <c r="AC24" s="120"/>
-      <c r="AD24" s="120"/>
-      <c r="AE24" s="120"/>
-      <c r="AF24" s="120"/>
-      <c r="AG24" s="125"/>
-      <c r="AH24" s="125"/>
-      <c r="AI24" s="125"/>
-      <c r="AJ24" s="125"/>
-      <c r="AK24" s="125"/>
-      <c r="AL24" s="125"/>
-      <c r="AM24" s="125"/>
-      <c r="AN24" s="125"/>
-      <c r="AO24" s="125"/>
-      <c r="AP24" s="125"/>
-      <c r="AQ24" s="125"/>
-      <c r="AR24" s="125"/>
-      <c r="AS24" s="125"/>
-      <c r="AT24" s="125"/>
-      <c r="AU24" s="125"/>
-      <c r="AV24" s="125"/>
-      <c r="AW24" s="125"/>
-      <c r="AX24" s="125"/>
-      <c r="AY24" s="125"/>
-      <c r="AZ24" s="125"/>
-      <c r="BA24" s="126"/>
+      <c r="V24" s="77"/>
+      <c r="W24" s="77"/>
+      <c r="X24" s="77"/>
+      <c r="Y24" s="77"/>
+      <c r="Z24" s="77"/>
+      <c r="AA24" s="77"/>
+      <c r="AB24" s="77"/>
+      <c r="AC24" s="77"/>
+      <c r="AD24" s="77"/>
+      <c r="AE24" s="77"/>
+      <c r="AF24" s="77"/>
+      <c r="AG24" s="82"/>
+      <c r="AH24" s="82"/>
+      <c r="AI24" s="82"/>
+      <c r="AJ24" s="82"/>
+      <c r="AK24" s="82"/>
+      <c r="AL24" s="82"/>
+      <c r="AM24" s="82"/>
+      <c r="AN24" s="82"/>
+      <c r="AO24" s="82"/>
+      <c r="AP24" s="82"/>
+      <c r="AQ24" s="82"/>
+      <c r="AR24" s="82"/>
+      <c r="AS24" s="82"/>
+      <c r="AT24" s="82"/>
+      <c r="AU24" s="82"/>
+      <c r="AV24" s="82"/>
+      <c r="AW24" s="82"/>
+      <c r="AX24" s="82"/>
+      <c r="AY24" s="82"/>
+      <c r="AZ24" s="82"/>
+      <c r="BA24" s="83"/>
       <c r="BB24" s="15"/>
       <c r="BC24" s="15"/>
       <c r="BD24" s="15"/>
@@ -3812,7 +3812,7 @@
       <c r="BQ24" s="14"/>
       <c r="BR24" s="15"/>
     </row>
-    <row r="25" spans="3:70" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.65">
+    <row r="25" spans="3:70" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="C25" s="15"/>
       <c r="D25" s="17"/>
       <c r="E25" s="15"/>
@@ -3831,41 +3831,41 @@
       <c r="R25" s="15"/>
       <c r="S25" s="15"/>
       <c r="T25" s="15"/>
-      <c r="U25" s="119" t="s">
+      <c r="U25" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="V25" s="120"/>
-      <c r="W25" s="120"/>
-      <c r="X25" s="120"/>
-      <c r="Y25" s="120"/>
-      <c r="Z25" s="120"/>
-      <c r="AA25" s="120"/>
-      <c r="AB25" s="120"/>
-      <c r="AC25" s="120"/>
-      <c r="AD25" s="120"/>
-      <c r="AE25" s="120"/>
-      <c r="AF25" s="120"/>
-      <c r="AG25" s="125"/>
-      <c r="AH25" s="125"/>
-      <c r="AI25" s="125"/>
-      <c r="AJ25" s="125"/>
-      <c r="AK25" s="125"/>
-      <c r="AL25" s="125"/>
-      <c r="AM25" s="125"/>
-      <c r="AN25" s="125"/>
-      <c r="AO25" s="125"/>
-      <c r="AP25" s="125"/>
-      <c r="AQ25" s="125"/>
-      <c r="AR25" s="125"/>
-      <c r="AS25" s="125"/>
-      <c r="AT25" s="125"/>
-      <c r="AU25" s="125"/>
-      <c r="AV25" s="125"/>
-      <c r="AW25" s="125"/>
-      <c r="AX25" s="125"/>
-      <c r="AY25" s="125"/>
-      <c r="AZ25" s="125"/>
-      <c r="BA25" s="126"/>
+      <c r="V25" s="77"/>
+      <c r="W25" s="77"/>
+      <c r="X25" s="77"/>
+      <c r="Y25" s="77"/>
+      <c r="Z25" s="77"/>
+      <c r="AA25" s="77"/>
+      <c r="AB25" s="77"/>
+      <c r="AC25" s="77"/>
+      <c r="AD25" s="77"/>
+      <c r="AE25" s="77"/>
+      <c r="AF25" s="77"/>
+      <c r="AG25" s="82"/>
+      <c r="AH25" s="82"/>
+      <c r="AI25" s="82"/>
+      <c r="AJ25" s="82"/>
+      <c r="AK25" s="82"/>
+      <c r="AL25" s="82"/>
+      <c r="AM25" s="82"/>
+      <c r="AN25" s="82"/>
+      <c r="AO25" s="82"/>
+      <c r="AP25" s="82"/>
+      <c r="AQ25" s="82"/>
+      <c r="AR25" s="82"/>
+      <c r="AS25" s="82"/>
+      <c r="AT25" s="82"/>
+      <c r="AU25" s="82"/>
+      <c r="AV25" s="82"/>
+      <c r="AW25" s="82"/>
+      <c r="AX25" s="82"/>
+      <c r="AY25" s="82"/>
+      <c r="AZ25" s="82"/>
+      <c r="BA25" s="83"/>
       <c r="BB25" s="15"/>
       <c r="BC25" s="15"/>
       <c r="BD25" s="15"/>
@@ -3884,7 +3884,7 @@
       <c r="BQ25" s="14"/>
       <c r="BR25" s="15"/>
     </row>
-    <row r="26" spans="3:70" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.65">
+    <row r="26" spans="3:70" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="C26" s="15"/>
       <c r="D26" s="17"/>
       <c r="E26" s="15"/>
@@ -3903,41 +3903,41 @@
       <c r="R26" s="15"/>
       <c r="S26" s="15"/>
       <c r="T26" s="15"/>
-      <c r="U26" s="119" t="s">
+      <c r="U26" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="V26" s="120"/>
-      <c r="W26" s="120"/>
-      <c r="X26" s="120"/>
-      <c r="Y26" s="120"/>
-      <c r="Z26" s="120"/>
-      <c r="AA26" s="120"/>
-      <c r="AB26" s="120"/>
-      <c r="AC26" s="120"/>
-      <c r="AD26" s="120"/>
-      <c r="AE26" s="120"/>
-      <c r="AF26" s="120"/>
-      <c r="AG26" s="125"/>
-      <c r="AH26" s="125"/>
-      <c r="AI26" s="125"/>
-      <c r="AJ26" s="125"/>
-      <c r="AK26" s="125"/>
-      <c r="AL26" s="125"/>
-      <c r="AM26" s="125"/>
-      <c r="AN26" s="125"/>
-      <c r="AO26" s="125"/>
-      <c r="AP26" s="125"/>
-      <c r="AQ26" s="125"/>
-      <c r="AR26" s="125"/>
-      <c r="AS26" s="125"/>
-      <c r="AT26" s="125"/>
-      <c r="AU26" s="125"/>
-      <c r="AV26" s="125"/>
-      <c r="AW26" s="125"/>
-      <c r="AX26" s="125"/>
-      <c r="AY26" s="125"/>
-      <c r="AZ26" s="125"/>
-      <c r="BA26" s="126"/>
+      <c r="V26" s="77"/>
+      <c r="W26" s="77"/>
+      <c r="X26" s="77"/>
+      <c r="Y26" s="77"/>
+      <c r="Z26" s="77"/>
+      <c r="AA26" s="77"/>
+      <c r="AB26" s="77"/>
+      <c r="AC26" s="77"/>
+      <c r="AD26" s="77"/>
+      <c r="AE26" s="77"/>
+      <c r="AF26" s="77"/>
+      <c r="AG26" s="82"/>
+      <c r="AH26" s="82"/>
+      <c r="AI26" s="82"/>
+      <c r="AJ26" s="82"/>
+      <c r="AK26" s="82"/>
+      <c r="AL26" s="82"/>
+      <c r="AM26" s="82"/>
+      <c r="AN26" s="82"/>
+      <c r="AO26" s="82"/>
+      <c r="AP26" s="82"/>
+      <c r="AQ26" s="82"/>
+      <c r="AR26" s="82"/>
+      <c r="AS26" s="82"/>
+      <c r="AT26" s="82"/>
+      <c r="AU26" s="82"/>
+      <c r="AV26" s="82"/>
+      <c r="AW26" s="82"/>
+      <c r="AX26" s="82"/>
+      <c r="AY26" s="82"/>
+      <c r="AZ26" s="82"/>
+      <c r="BA26" s="83"/>
       <c r="BB26" s="15"/>
       <c r="BC26" s="15"/>
       <c r="BD26" s="15"/>
@@ -3956,7 +3956,7 @@
       <c r="BQ26" s="14"/>
       <c r="BR26" s="15"/>
     </row>
-    <row r="27" spans="3:70" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.65">
+    <row r="27" spans="3:70" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="C27" s="15"/>
       <c r="D27" s="17"/>
       <c r="E27" s="15"/>
@@ -3975,41 +3975,41 @@
       <c r="R27" s="15"/>
       <c r="S27" s="15"/>
       <c r="T27" s="15"/>
-      <c r="U27" s="119" t="s">
+      <c r="U27" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="V27" s="120"/>
-      <c r="W27" s="120"/>
-      <c r="X27" s="120"/>
-      <c r="Y27" s="120"/>
-      <c r="Z27" s="120"/>
-      <c r="AA27" s="120"/>
-      <c r="AB27" s="120"/>
-      <c r="AC27" s="120"/>
-      <c r="AD27" s="120"/>
-      <c r="AE27" s="120"/>
-      <c r="AF27" s="120"/>
-      <c r="AG27" s="129"/>
-      <c r="AH27" s="129"/>
-      <c r="AI27" s="129"/>
-      <c r="AJ27" s="129"/>
-      <c r="AK27" s="129"/>
-      <c r="AL27" s="129"/>
-      <c r="AM27" s="129"/>
-      <c r="AN27" s="129"/>
-      <c r="AO27" s="129"/>
-      <c r="AP27" s="129"/>
-      <c r="AQ27" s="129"/>
-      <c r="AR27" s="129"/>
-      <c r="AS27" s="129"/>
-      <c r="AT27" s="129"/>
-      <c r="AU27" s="129"/>
-      <c r="AV27" s="129"/>
-      <c r="AW27" s="129"/>
-      <c r="AX27" s="129"/>
-      <c r="AY27" s="129"/>
-      <c r="AZ27" s="129"/>
-      <c r="BA27" s="130"/>
+      <c r="V27" s="77"/>
+      <c r="W27" s="77"/>
+      <c r="X27" s="77"/>
+      <c r="Y27" s="77"/>
+      <c r="Z27" s="77"/>
+      <c r="AA27" s="77"/>
+      <c r="AB27" s="77"/>
+      <c r="AC27" s="77"/>
+      <c r="AD27" s="77"/>
+      <c r="AE27" s="77"/>
+      <c r="AF27" s="77"/>
+      <c r="AG27" s="86"/>
+      <c r="AH27" s="86"/>
+      <c r="AI27" s="86"/>
+      <c r="AJ27" s="86"/>
+      <c r="AK27" s="86"/>
+      <c r="AL27" s="86"/>
+      <c r="AM27" s="86"/>
+      <c r="AN27" s="86"/>
+      <c r="AO27" s="86"/>
+      <c r="AP27" s="86"/>
+      <c r="AQ27" s="86"/>
+      <c r="AR27" s="86"/>
+      <c r="AS27" s="86"/>
+      <c r="AT27" s="86"/>
+      <c r="AU27" s="86"/>
+      <c r="AV27" s="86"/>
+      <c r="AW27" s="86"/>
+      <c r="AX27" s="86"/>
+      <c r="AY27" s="86"/>
+      <c r="AZ27" s="86"/>
+      <c r="BA27" s="87"/>
       <c r="BB27" s="15"/>
       <c r="BC27" s="15"/>
       <c r="BD27" s="15"/>
@@ -4028,7 +4028,7 @@
       <c r="BQ27" s="14"/>
       <c r="BR27" s="15"/>
     </row>
-    <row r="28" spans="3:70" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.65">
+    <row r="28" spans="3:70" s="16" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="C28" s="15"/>
       <c r="D28" s="17"/>
       <c r="E28" s="15"/>
@@ -4047,41 +4047,41 @@
       <c r="R28" s="15"/>
       <c r="S28" s="15"/>
       <c r="T28" s="15"/>
-      <c r="U28" s="119" t="s">
+      <c r="U28" s="76" t="s">
         <v>44</v>
       </c>
-      <c r="V28" s="120"/>
-      <c r="W28" s="120"/>
-      <c r="X28" s="120"/>
-      <c r="Y28" s="120"/>
-      <c r="Z28" s="120"/>
-      <c r="AA28" s="120"/>
-      <c r="AB28" s="120"/>
-      <c r="AC28" s="120"/>
-      <c r="AD28" s="120"/>
-      <c r="AE28" s="120"/>
-      <c r="AF28" s="120"/>
-      <c r="AG28" s="125"/>
-      <c r="AH28" s="125"/>
-      <c r="AI28" s="125"/>
-      <c r="AJ28" s="125"/>
-      <c r="AK28" s="125"/>
-      <c r="AL28" s="125"/>
-      <c r="AM28" s="125"/>
-      <c r="AN28" s="125"/>
-      <c r="AO28" s="125"/>
-      <c r="AP28" s="125"/>
-      <c r="AQ28" s="125"/>
-      <c r="AR28" s="125"/>
-      <c r="AS28" s="125"/>
-      <c r="AT28" s="125"/>
-      <c r="AU28" s="125"/>
-      <c r="AV28" s="125"/>
-      <c r="AW28" s="125"/>
-      <c r="AX28" s="125"/>
-      <c r="AY28" s="125"/>
-      <c r="AZ28" s="125"/>
-      <c r="BA28" s="126"/>
+      <c r="V28" s="77"/>
+      <c r="W28" s="77"/>
+      <c r="X28" s="77"/>
+      <c r="Y28" s="77"/>
+      <c r="Z28" s="77"/>
+      <c r="AA28" s="77"/>
+      <c r="AB28" s="77"/>
+      <c r="AC28" s="77"/>
+      <c r="AD28" s="77"/>
+      <c r="AE28" s="77"/>
+      <c r="AF28" s="77"/>
+      <c r="AG28" s="82"/>
+      <c r="AH28" s="82"/>
+      <c r="AI28" s="82"/>
+      <c r="AJ28" s="82"/>
+      <c r="AK28" s="82"/>
+      <c r="AL28" s="82"/>
+      <c r="AM28" s="82"/>
+      <c r="AN28" s="82"/>
+      <c r="AO28" s="82"/>
+      <c r="AP28" s="82"/>
+      <c r="AQ28" s="82"/>
+      <c r="AR28" s="82"/>
+      <c r="AS28" s="82"/>
+      <c r="AT28" s="82"/>
+      <c r="AU28" s="82"/>
+      <c r="AV28" s="82"/>
+      <c r="AW28" s="82"/>
+      <c r="AX28" s="82"/>
+      <c r="AY28" s="82"/>
+      <c r="AZ28" s="82"/>
+      <c r="BA28" s="83"/>
       <c r="BB28" s="15"/>
       <c r="BC28" s="15"/>
       <c r="BD28" s="15"/>
@@ -4100,7 +4100,7 @@
       <c r="BQ28" s="14"/>
       <c r="BR28" s="15"/>
     </row>
-    <row r="29" spans="3:70" s="16" customFormat="1" ht="21.4" thickBot="1" x14ac:dyDescent="0.7">
+    <row r="29" spans="3:70" s="16" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C29" s="15"/>
       <c r="D29" s="12"/>
       <c r="E29" s="11"/>
@@ -4119,41 +4119,41 @@
       <c r="R29" s="11"/>
       <c r="S29" s="11"/>
       <c r="T29" s="11"/>
-      <c r="U29" s="127" t="s">
+      <c r="U29" s="84" t="s">
         <v>5</v>
       </c>
-      <c r="V29" s="128"/>
-      <c r="W29" s="128"/>
-      <c r="X29" s="128"/>
-      <c r="Y29" s="128"/>
-      <c r="Z29" s="128"/>
-      <c r="AA29" s="128"/>
-      <c r="AB29" s="128"/>
-      <c r="AC29" s="128"/>
-      <c r="AD29" s="128"/>
-      <c r="AE29" s="128"/>
-      <c r="AF29" s="128"/>
-      <c r="AG29" s="131"/>
-      <c r="AH29" s="131"/>
-      <c r="AI29" s="131"/>
-      <c r="AJ29" s="131"/>
-      <c r="AK29" s="131"/>
-      <c r="AL29" s="131"/>
-      <c r="AM29" s="131"/>
-      <c r="AN29" s="131"/>
-      <c r="AO29" s="131"/>
-      <c r="AP29" s="131"/>
-      <c r="AQ29" s="131"/>
-      <c r="AR29" s="131"/>
-      <c r="AS29" s="131"/>
-      <c r="AT29" s="131"/>
-      <c r="AU29" s="131"/>
-      <c r="AV29" s="131"/>
-      <c r="AW29" s="131"/>
-      <c r="AX29" s="131"/>
-      <c r="AY29" s="131"/>
-      <c r="AZ29" s="131"/>
-      <c r="BA29" s="132"/>
+      <c r="V29" s="85"/>
+      <c r="W29" s="85"/>
+      <c r="X29" s="85"/>
+      <c r="Y29" s="85"/>
+      <c r="Z29" s="85"/>
+      <c r="AA29" s="85"/>
+      <c r="AB29" s="85"/>
+      <c r="AC29" s="85"/>
+      <c r="AD29" s="85"/>
+      <c r="AE29" s="85"/>
+      <c r="AF29" s="85"/>
+      <c r="AG29" s="88"/>
+      <c r="AH29" s="88"/>
+      <c r="AI29" s="88"/>
+      <c r="AJ29" s="88"/>
+      <c r="AK29" s="88"/>
+      <c r="AL29" s="88"/>
+      <c r="AM29" s="88"/>
+      <c r="AN29" s="88"/>
+      <c r="AO29" s="88"/>
+      <c r="AP29" s="88"/>
+      <c r="AQ29" s="88"/>
+      <c r="AR29" s="88"/>
+      <c r="AS29" s="88"/>
+      <c r="AT29" s="88"/>
+      <c r="AU29" s="88"/>
+      <c r="AV29" s="88"/>
+      <c r="AW29" s="88"/>
+      <c r="AX29" s="88"/>
+      <c r="AY29" s="88"/>
+      <c r="AZ29" s="88"/>
+      <c r="BA29" s="89"/>
       <c r="BB29" s="11"/>
       <c r="BC29" s="11"/>
       <c r="BD29" s="11"/>
@@ -4172,7 +4172,7 @@
       <c r="BQ29" s="10"/>
       <c r="BR29" s="15"/>
     </row>
-    <row r="30" spans="3:70" x14ac:dyDescent="0.35">
+    <row r="30" spans="3:70" x14ac:dyDescent="0.2">
       <c r="C30" s="11"/>
       <c r="D30" s="12"/>
       <c r="E30" s="11"/>
@@ -4242,7 +4242,7 @@
       <c r="BQ30" s="10"/>
       <c r="BR30" s="11"/>
     </row>
-    <row r="31" spans="3:70" x14ac:dyDescent="0.35">
+    <row r="31" spans="3:70" x14ac:dyDescent="0.2">
       <c r="C31" s="11"/>
       <c r="D31" s="12"/>
       <c r="E31" s="11"/>
@@ -4312,7 +4312,7 @@
       <c r="BQ31" s="10"/>
       <c r="BR31" s="11"/>
     </row>
-    <row r="32" spans="3:70" x14ac:dyDescent="0.35">
+    <row r="32" spans="3:70" x14ac:dyDescent="0.2">
       <c r="C32" s="11"/>
       <c r="D32" s="12"/>
       <c r="E32" s="11"/>
@@ -4382,7 +4382,7 @@
       <c r="BQ32" s="10"/>
       <c r="BR32" s="11"/>
     </row>
-    <row r="33" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:72" x14ac:dyDescent="0.2">
       <c r="C33" s="11"/>
       <c r="D33" s="12"/>
       <c r="E33" s="11"/>
@@ -4452,7 +4452,7 @@
       <c r="BQ33" s="10"/>
       <c r="BR33" s="11"/>
     </row>
-    <row r="34" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:72" x14ac:dyDescent="0.2">
       <c r="C34" s="11"/>
       <c r="D34" s="12"/>
       <c r="E34" s="11"/>
@@ -4522,7 +4522,7 @@
       <c r="BQ34" s="10"/>
       <c r="BR34" s="11"/>
     </row>
-    <row r="35" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:72" x14ac:dyDescent="0.2">
       <c r="C35" s="11"/>
       <c r="D35" s="12"/>
       <c r="E35" s="11"/>
@@ -4592,7 +4592,7 @@
       <c r="BQ35" s="10"/>
       <c r="BR35" s="11"/>
     </row>
-    <row r="36" spans="1:72" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:72" x14ac:dyDescent="0.2">
       <c r="C36" s="11"/>
       <c r="D36" s="12"/>
       <c r="E36" s="11"/>
@@ -4662,7 +4662,7 @@
       <c r="BQ36" s="10"/>
       <c r="BR36" s="11"/>
     </row>
-    <row r="37" spans="1:72" ht="10.9" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:72" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C37" s="11"/>
       <c r="D37" s="12"/>
       <c r="E37" s="18"/>
@@ -4732,50 +4732,50 @@
       <c r="BQ37" s="10"/>
       <c r="BR37" s="11"/>
     </row>
-    <row r="39" spans="1:72" x14ac:dyDescent="0.35">
-      <c r="A39" s="67" t="s">
+    <row r="39" spans="1:72" x14ac:dyDescent="0.2">
+      <c r="A39" s="91" t="s">
         <v>6</v>
       </c>
-      <c r="B39" s="67"/>
-      <c r="C39" s="67"/>
-      <c r="D39" s="67"/>
+      <c r="B39" s="91"/>
+      <c r="C39" s="91"/>
+      <c r="D39" s="91"/>
       <c r="E39" s="64" t="s">
         <v>19</v>
       </c>
       <c r="F39" s="65"/>
       <c r="G39" s="65"/>
       <c r="H39" s="66"/>
-      <c r="I39" s="67" t="s">
+      <c r="I39" s="91" t="s">
         <v>41</v>
       </c>
-      <c r="J39" s="67"/>
-      <c r="K39" s="67"/>
-      <c r="L39" s="67"/>
-      <c r="M39" s="67"/>
+      <c r="J39" s="91"/>
+      <c r="K39" s="91"/>
+      <c r="L39" s="91"/>
+      <c r="M39" s="91"/>
       <c r="N39" s="64" t="s">
         <v>7</v>
       </c>
       <c r="O39" s="66"/>
-      <c r="P39" s="67" t="s">
+      <c r="P39" s="91" t="s">
         <v>8</v>
       </c>
-      <c r="Q39" s="67"/>
-      <c r="R39" s="67"/>
-      <c r="S39" s="67"/>
-      <c r="T39" s="67" t="s">
+      <c r="Q39" s="91"/>
+      <c r="R39" s="91"/>
+      <c r="S39" s="91"/>
+      <c r="T39" s="91" t="s">
         <v>9</v>
       </c>
-      <c r="U39" s="67"/>
-      <c r="V39" s="67"/>
-      <c r="W39" s="67"/>
-      <c r="X39" s="67" t="s">
+      <c r="U39" s="91"/>
+      <c r="V39" s="91"/>
+      <c r="W39" s="91"/>
+      <c r="X39" s="91" t="s">
         <v>40</v>
       </c>
-      <c r="Y39" s="67"/>
-      <c r="Z39" s="67"/>
-      <c r="AA39" s="67"/>
-      <c r="AB39" s="67"/>
-      <c r="AC39" s="67"/>
+      <c r="Y39" s="91"/>
+      <c r="Z39" s="91"/>
+      <c r="AA39" s="91"/>
+      <c r="AB39" s="91"/>
+      <c r="AC39" s="91"/>
       <c r="AD39" s="64" t="s">
         <v>10</v>
       </c>
@@ -4786,11 +4786,11 @@
       <c r="AI39" s="65"/>
       <c r="AJ39" s="65"/>
       <c r="AK39" s="66"/>
-      <c r="AL39" s="67" t="s">
+      <c r="AL39" s="91" t="s">
         <v>37</v>
       </c>
-      <c r="AM39" s="67"/>
-      <c r="AN39" s="67"/>
+      <c r="AM39" s="91"/>
+      <c r="AN39" s="91"/>
       <c r="AO39" s="64" t="s">
         <v>18</v>
       </c>
@@ -4799,639 +4799,622 @@
       <c r="AR39" s="65"/>
       <c r="AS39" s="65"/>
       <c r="AT39" s="66"/>
-      <c r="AU39" s="67" t="s">
+      <c r="AU39" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="AV39" s="67"/>
-      <c r="AW39" s="67"/>
-      <c r="AX39" s="67"/>
-      <c r="AY39" s="67"/>
-      <c r="AZ39" s="67" t="s">
+      <c r="AV39" s="91"/>
+      <c r="AW39" s="91"/>
+      <c r="AX39" s="91"/>
+      <c r="AY39" s="91"/>
+      <c r="AZ39" s="91" t="s">
         <v>12</v>
       </c>
-      <c r="BA39" s="67"/>
-      <c r="BB39" s="67"/>
-      <c r="BC39" s="67"/>
-      <c r="BD39" s="67"/>
-      <c r="BE39" s="67" t="s">
+      <c r="BA39" s="91"/>
+      <c r="BB39" s="91"/>
+      <c r="BC39" s="91"/>
+      <c r="BD39" s="91"/>
+      <c r="BE39" s="91" t="s">
         <v>36</v>
       </c>
-      <c r="BF39" s="67"/>
-      <c r="BG39" s="67"/>
-      <c r="BH39" s="67"/>
-      <c r="BI39" s="67"/>
-      <c r="BJ39" s="67" t="s">
+      <c r="BF39" s="91"/>
+      <c r="BG39" s="91"/>
+      <c r="BH39" s="91"/>
+      <c r="BI39" s="91"/>
+      <c r="BJ39" s="91" t="s">
         <v>20</v>
       </c>
-      <c r="BK39" s="67"/>
-      <c r="BL39" s="67" t="s">
+      <c r="BK39" s="91"/>
+      <c r="BL39" s="91" t="s">
         <v>35</v>
       </c>
-      <c r="BM39" s="67"/>
-      <c r="BN39" s="67"/>
-      <c r="BO39" s="67"/>
-      <c r="BP39" s="67"/>
-      <c r="BQ39" s="67"/>
-      <c r="BR39" s="67"/>
-      <c r="BS39" s="67"/>
-      <c r="BT39" s="67"/>
-    </row>
-    <row r="40" spans="1:72" ht="11.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="68"/>
-      <c r="B40" s="68"/>
-      <c r="C40" s="68"/>
-      <c r="D40" s="68"/>
-      <c r="E40" s="69"/>
-      <c r="F40" s="116"/>
-      <c r="G40" s="116"/>
-      <c r="H40" s="70"/>
-      <c r="I40" s="68"/>
-      <c r="J40" s="68"/>
-      <c r="K40" s="68"/>
-      <c r="L40" s="68"/>
-      <c r="M40" s="68"/>
-      <c r="N40" s="69"/>
-      <c r="O40" s="70"/>
-      <c r="P40" s="68"/>
-      <c r="Q40" s="68"/>
-      <c r="R40" s="68"/>
-      <c r="S40" s="68"/>
-      <c r="T40" s="68"/>
-      <c r="U40" s="68"/>
-      <c r="V40" s="68"/>
-      <c r="W40" s="68"/>
-      <c r="X40" s="133"/>
-      <c r="Y40" s="134"/>
-      <c r="Z40" s="134"/>
-      <c r="AA40" s="134"/>
-      <c r="AB40" s="134"/>
-      <c r="AC40" s="135"/>
-      <c r="AD40" s="69"/>
-      <c r="AE40" s="116"/>
-      <c r="AF40" s="116"/>
-      <c r="AG40" s="116"/>
-      <c r="AH40" s="116"/>
-      <c r="AI40" s="116"/>
-      <c r="AJ40" s="116"/>
-      <c r="AK40" s="70"/>
-      <c r="AL40" s="68"/>
-      <c r="AM40" s="68"/>
-      <c r="AN40" s="68"/>
-      <c r="AO40" s="107"/>
-      <c r="AP40" s="108"/>
-      <c r="AQ40" s="108"/>
-      <c r="AR40" s="108"/>
-      <c r="AS40" s="108"/>
-      <c r="AT40" s="109"/>
-      <c r="AU40" s="68"/>
-      <c r="AV40" s="68"/>
-      <c r="AW40" s="68"/>
-      <c r="AX40" s="68"/>
-      <c r="AY40" s="68"/>
-      <c r="AZ40" s="68"/>
-      <c r="BA40" s="68"/>
-      <c r="BB40" s="68"/>
-      <c r="BC40" s="68"/>
-      <c r="BD40" s="68"/>
-      <c r="BE40" s="68"/>
-      <c r="BF40" s="68"/>
-      <c r="BG40" s="68"/>
-      <c r="BH40" s="68"/>
-      <c r="BI40" s="68"/>
-      <c r="BJ40" s="68"/>
-      <c r="BK40" s="68"/>
-      <c r="BL40" s="98"/>
-      <c r="BM40" s="99"/>
-      <c r="BN40" s="99"/>
-      <c r="BO40" s="99"/>
-      <c r="BP40" s="99"/>
-      <c r="BQ40" s="99"/>
-      <c r="BR40" s="99"/>
-      <c r="BS40" s="99"/>
-      <c r="BT40" s="100"/>
-    </row>
-    <row r="41" spans="1:72" x14ac:dyDescent="0.35">
-      <c r="A41" s="68"/>
-      <c r="B41" s="68"/>
-      <c r="C41" s="68"/>
-      <c r="D41" s="68"/>
-      <c r="E41" s="71"/>
-      <c r="F41" s="117"/>
-      <c r="G41" s="117"/>
+      <c r="BM39" s="91"/>
+      <c r="BN39" s="91"/>
+      <c r="BO39" s="91"/>
+      <c r="BP39" s="91"/>
+      <c r="BQ39" s="91"/>
+      <c r="BR39" s="91"/>
+      <c r="BS39" s="91"/>
+      <c r="BT39" s="91"/>
+    </row>
+    <row r="40" spans="1:72" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="90"/>
+      <c r="B40" s="90"/>
+      <c r="C40" s="90"/>
+      <c r="D40" s="90"/>
+      <c r="E40" s="67"/>
+      <c r="F40" s="68"/>
+      <c r="G40" s="68"/>
+      <c r="H40" s="69"/>
+      <c r="I40" s="90"/>
+      <c r="J40" s="90"/>
+      <c r="K40" s="90"/>
+      <c r="L40" s="90"/>
+      <c r="M40" s="90"/>
+      <c r="N40" s="67"/>
+      <c r="O40" s="69"/>
+      <c r="P40" s="90"/>
+      <c r="Q40" s="90"/>
+      <c r="R40" s="90"/>
+      <c r="S40" s="90"/>
+      <c r="T40" s="90"/>
+      <c r="U40" s="90"/>
+      <c r="V40" s="90"/>
+      <c r="W40" s="90"/>
+      <c r="X40" s="92"/>
+      <c r="Y40" s="93"/>
+      <c r="Z40" s="93"/>
+      <c r="AA40" s="93"/>
+      <c r="AB40" s="93"/>
+      <c r="AC40" s="94"/>
+      <c r="AD40" s="67"/>
+      <c r="AE40" s="68"/>
+      <c r="AF40" s="68"/>
+      <c r="AG40" s="68"/>
+      <c r="AH40" s="68"/>
+      <c r="AI40" s="68"/>
+      <c r="AJ40" s="68"/>
+      <c r="AK40" s="69"/>
+      <c r="AL40" s="90"/>
+      <c r="AM40" s="90"/>
+      <c r="AN40" s="90"/>
+      <c r="AO40" s="110"/>
+      <c r="AP40" s="111"/>
+      <c r="AQ40" s="111"/>
+      <c r="AR40" s="111"/>
+      <c r="AS40" s="111"/>
+      <c r="AT40" s="112"/>
+      <c r="AU40" s="90"/>
+      <c r="AV40" s="90"/>
+      <c r="AW40" s="90"/>
+      <c r="AX40" s="90"/>
+      <c r="AY40" s="90"/>
+      <c r="AZ40" s="90"/>
+      <c r="BA40" s="90"/>
+      <c r="BB40" s="90"/>
+      <c r="BC40" s="90"/>
+      <c r="BD40" s="90"/>
+      <c r="BE40" s="90"/>
+      <c r="BF40" s="90"/>
+      <c r="BG40" s="90"/>
+      <c r="BH40" s="90"/>
+      <c r="BI40" s="90"/>
+      <c r="BJ40" s="90"/>
+      <c r="BK40" s="90"/>
+      <c r="BL40" s="101"/>
+      <c r="BM40" s="102"/>
+      <c r="BN40" s="102"/>
+      <c r="BO40" s="102"/>
+      <c r="BP40" s="102"/>
+      <c r="BQ40" s="102"/>
+      <c r="BR40" s="102"/>
+      <c r="BS40" s="102"/>
+      <c r="BT40" s="103"/>
+    </row>
+    <row r="41" spans="1:72" x14ac:dyDescent="0.2">
+      <c r="A41" s="90"/>
+      <c r="B41" s="90"/>
+      <c r="C41" s="90"/>
+      <c r="D41" s="90"/>
+      <c r="E41" s="70"/>
+      <c r="F41" s="71"/>
+      <c r="G41" s="71"/>
       <c r="H41" s="72"/>
-      <c r="I41" s="68"/>
-      <c r="J41" s="68"/>
-      <c r="K41" s="68"/>
-      <c r="L41" s="68"/>
-      <c r="M41" s="68"/>
-      <c r="N41" s="71"/>
+      <c r="I41" s="90"/>
+      <c r="J41" s="90"/>
+      <c r="K41" s="90"/>
+      <c r="L41" s="90"/>
+      <c r="M41" s="90"/>
+      <c r="N41" s="70"/>
       <c r="O41" s="72"/>
-      <c r="P41" s="68"/>
-      <c r="Q41" s="68"/>
-      <c r="R41" s="68"/>
-      <c r="S41" s="68"/>
-      <c r="T41" s="68"/>
-      <c r="U41" s="68"/>
-      <c r="V41" s="68"/>
-      <c r="W41" s="68"/>
-      <c r="X41" s="136"/>
-      <c r="Y41" s="137"/>
-      <c r="Z41" s="137"/>
-      <c r="AA41" s="137"/>
-      <c r="AB41" s="137"/>
-      <c r="AC41" s="138"/>
-      <c r="AD41" s="71"/>
-      <c r="AE41" s="117"/>
-      <c r="AF41" s="117"/>
-      <c r="AG41" s="117"/>
-      <c r="AH41" s="117"/>
-      <c r="AI41" s="117"/>
-      <c r="AJ41" s="117"/>
+      <c r="P41" s="90"/>
+      <c r="Q41" s="90"/>
+      <c r="R41" s="90"/>
+      <c r="S41" s="90"/>
+      <c r="T41" s="90"/>
+      <c r="U41" s="90"/>
+      <c r="V41" s="90"/>
+      <c r="W41" s="90"/>
+      <c r="X41" s="95"/>
+      <c r="Y41" s="96"/>
+      <c r="Z41" s="96"/>
+      <c r="AA41" s="96"/>
+      <c r="AB41" s="96"/>
+      <c r="AC41" s="97"/>
+      <c r="AD41" s="70"/>
+      <c r="AE41" s="71"/>
+      <c r="AF41" s="71"/>
+      <c r="AG41" s="71"/>
+      <c r="AH41" s="71"/>
+      <c r="AI41" s="71"/>
+      <c r="AJ41" s="71"/>
       <c r="AK41" s="72"/>
-      <c r="AL41" s="68"/>
-      <c r="AM41" s="68"/>
-      <c r="AN41" s="68"/>
-      <c r="AO41" s="110"/>
-      <c r="AP41" s="111"/>
-      <c r="AQ41" s="111"/>
-      <c r="AR41" s="111"/>
-      <c r="AS41" s="111"/>
-      <c r="AT41" s="112"/>
-      <c r="AU41" s="68"/>
-      <c r="AV41" s="68"/>
-      <c r="AW41" s="68"/>
-      <c r="AX41" s="68"/>
-      <c r="AY41" s="68"/>
-      <c r="AZ41" s="68"/>
-      <c r="BA41" s="68"/>
-      <c r="BB41" s="68"/>
-      <c r="BC41" s="68"/>
-      <c r="BD41" s="68"/>
-      <c r="BE41" s="68"/>
-      <c r="BF41" s="68"/>
-      <c r="BG41" s="68"/>
-      <c r="BH41" s="68"/>
-      <c r="BI41" s="68"/>
-      <c r="BJ41" s="68"/>
-      <c r="BK41" s="68"/>
-      <c r="BL41" s="101"/>
-      <c r="BM41" s="102"/>
-      <c r="BN41" s="102"/>
-      <c r="BO41" s="102"/>
-      <c r="BP41" s="102"/>
-      <c r="BQ41" s="102"/>
-      <c r="BR41" s="102"/>
-      <c r="BS41" s="102"/>
-      <c r="BT41" s="103"/>
-    </row>
-    <row r="42" spans="1:72" x14ac:dyDescent="0.35">
-      <c r="A42" s="68"/>
-      <c r="B42" s="68"/>
-      <c r="C42" s="68"/>
-      <c r="D42" s="68"/>
+      <c r="AL41" s="90"/>
+      <c r="AM41" s="90"/>
+      <c r="AN41" s="90"/>
+      <c r="AO41" s="113"/>
+      <c r="AP41" s="114"/>
+      <c r="AQ41" s="114"/>
+      <c r="AR41" s="114"/>
+      <c r="AS41" s="114"/>
+      <c r="AT41" s="115"/>
+      <c r="AU41" s="90"/>
+      <c r="AV41" s="90"/>
+      <c r="AW41" s="90"/>
+      <c r="AX41" s="90"/>
+      <c r="AY41" s="90"/>
+      <c r="AZ41" s="90"/>
+      <c r="BA41" s="90"/>
+      <c r="BB41" s="90"/>
+      <c r="BC41" s="90"/>
+      <c r="BD41" s="90"/>
+      <c r="BE41" s="90"/>
+      <c r="BF41" s="90"/>
+      <c r="BG41" s="90"/>
+      <c r="BH41" s="90"/>
+      <c r="BI41" s="90"/>
+      <c r="BJ41" s="90"/>
+      <c r="BK41" s="90"/>
+      <c r="BL41" s="104"/>
+      <c r="BM41" s="105"/>
+      <c r="BN41" s="105"/>
+      <c r="BO41" s="105"/>
+      <c r="BP41" s="105"/>
+      <c r="BQ41" s="105"/>
+      <c r="BR41" s="105"/>
+      <c r="BS41" s="105"/>
+      <c r="BT41" s="106"/>
+    </row>
+    <row r="42" spans="1:72" x14ac:dyDescent="0.2">
+      <c r="A42" s="90"/>
+      <c r="B42" s="90"/>
+      <c r="C42" s="90"/>
+      <c r="D42" s="90"/>
       <c r="E42" s="73"/>
-      <c r="F42" s="118"/>
-      <c r="G42" s="118"/>
-      <c r="H42" s="74"/>
-      <c r="I42" s="68"/>
-      <c r="J42" s="68"/>
-      <c r="K42" s="68"/>
-      <c r="L42" s="68"/>
-      <c r="M42" s="68"/>
+      <c r="F42" s="74"/>
+      <c r="G42" s="74"/>
+      <c r="H42" s="75"/>
+      <c r="I42" s="90"/>
+      <c r="J42" s="90"/>
+      <c r="K42" s="90"/>
+      <c r="L42" s="90"/>
+      <c r="M42" s="90"/>
       <c r="N42" s="73"/>
-      <c r="O42" s="74"/>
-      <c r="P42" s="68"/>
-      <c r="Q42" s="68"/>
-      <c r="R42" s="68"/>
-      <c r="S42" s="68"/>
-      <c r="T42" s="68"/>
-      <c r="U42" s="68"/>
-      <c r="V42" s="68"/>
-      <c r="W42" s="68"/>
-      <c r="X42" s="139"/>
-      <c r="Y42" s="140"/>
-      <c r="Z42" s="140"/>
-      <c r="AA42" s="140"/>
-      <c r="AB42" s="140"/>
-      <c r="AC42" s="141"/>
+      <c r="O42" s="75"/>
+      <c r="P42" s="90"/>
+      <c r="Q42" s="90"/>
+      <c r="R42" s="90"/>
+      <c r="S42" s="90"/>
+      <c r="T42" s="90"/>
+      <c r="U42" s="90"/>
+      <c r="V42" s="90"/>
+      <c r="W42" s="90"/>
+      <c r="X42" s="98"/>
+      <c r="Y42" s="99"/>
+      <c r="Z42" s="99"/>
+      <c r="AA42" s="99"/>
+      <c r="AB42" s="99"/>
+      <c r="AC42" s="100"/>
       <c r="AD42" s="73"/>
-      <c r="AE42" s="118"/>
-      <c r="AF42" s="118"/>
-      <c r="AG42" s="118"/>
-      <c r="AH42" s="118"/>
-      <c r="AI42" s="118"/>
-      <c r="AJ42" s="118"/>
-      <c r="AK42" s="74"/>
-      <c r="AL42" s="68"/>
-      <c r="AM42" s="68"/>
-      <c r="AN42" s="68"/>
-      <c r="AO42" s="113"/>
-      <c r="AP42" s="114"/>
-      <c r="AQ42" s="114"/>
-      <c r="AR42" s="114"/>
-      <c r="AS42" s="114"/>
-      <c r="AT42" s="115"/>
-      <c r="AU42" s="68"/>
-      <c r="AV42" s="68"/>
-      <c r="AW42" s="68"/>
-      <c r="AX42" s="68"/>
-      <c r="AY42" s="68"/>
-      <c r="AZ42" s="68"/>
-      <c r="BA42" s="68"/>
-      <c r="BB42" s="68"/>
-      <c r="BC42" s="68"/>
-      <c r="BD42" s="68"/>
-      <c r="BE42" s="68"/>
-      <c r="BF42" s="68"/>
-      <c r="BG42" s="68"/>
-      <c r="BH42" s="68"/>
-      <c r="BI42" s="68"/>
-      <c r="BJ42" s="68"/>
-      <c r="BK42" s="68"/>
-      <c r="BL42" s="104"/>
-      <c r="BM42" s="105"/>
-      <c r="BN42" s="105"/>
-      <c r="BO42" s="105"/>
-      <c r="BP42" s="105"/>
-      <c r="BQ42" s="105"/>
-      <c r="BR42" s="105"/>
-      <c r="BS42" s="105"/>
-      <c r="BT42" s="106"/>
-    </row>
-    <row r="43" spans="1:72" ht="11.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="88" t="s">
+      <c r="AE42" s="74"/>
+      <c r="AF42" s="74"/>
+      <c r="AG42" s="74"/>
+      <c r="AH42" s="74"/>
+      <c r="AI42" s="74"/>
+      <c r="AJ42" s="74"/>
+      <c r="AK42" s="75"/>
+      <c r="AL42" s="90"/>
+      <c r="AM42" s="90"/>
+      <c r="AN42" s="90"/>
+      <c r="AO42" s="116"/>
+      <c r="AP42" s="117"/>
+      <c r="AQ42" s="117"/>
+      <c r="AR42" s="117"/>
+      <c r="AS42" s="117"/>
+      <c r="AT42" s="118"/>
+      <c r="AU42" s="90"/>
+      <c r="AV42" s="90"/>
+      <c r="AW42" s="90"/>
+      <c r="AX42" s="90"/>
+      <c r="AY42" s="90"/>
+      <c r="AZ42" s="90"/>
+      <c r="BA42" s="90"/>
+      <c r="BB42" s="90"/>
+      <c r="BC42" s="90"/>
+      <c r="BD42" s="90"/>
+      <c r="BE42" s="90"/>
+      <c r="BF42" s="90"/>
+      <c r="BG42" s="90"/>
+      <c r="BH42" s="90"/>
+      <c r="BI42" s="90"/>
+      <c r="BJ42" s="90"/>
+      <c r="BK42" s="90"/>
+      <c r="BL42" s="107"/>
+      <c r="BM42" s="108"/>
+      <c r="BN42" s="108"/>
+      <c r="BO42" s="108"/>
+      <c r="BP42" s="108"/>
+      <c r="BQ42" s="108"/>
+      <c r="BR42" s="108"/>
+      <c r="BS42" s="108"/>
+      <c r="BT42" s="109"/>
+    </row>
+    <row r="43" spans="1:72" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="120" t="s">
         <v>34</v>
       </c>
-      <c r="B43" s="89"/>
-      <c r="C43" s="63" t="s">
+      <c r="B43" s="121"/>
+      <c r="C43" s="119" t="s">
         <v>29</v>
       </c>
-      <c r="D43" s="63"/>
-      <c r="E43" s="63"/>
-      <c r="F43" s="63"/>
-      <c r="G43" s="88" t="s">
+      <c r="D43" s="119"/>
+      <c r="E43" s="119"/>
+      <c r="F43" s="119"/>
+      <c r="G43" s="120" t="s">
         <v>39</v>
       </c>
-      <c r="H43" s="90"/>
-      <c r="I43" s="90"/>
-      <c r="J43" s="90"/>
-      <c r="K43" s="89"/>
-      <c r="L43" s="86" t="s">
+      <c r="H43" s="122"/>
+      <c r="I43" s="122"/>
+      <c r="J43" s="122"/>
+      <c r="K43" s="121"/>
+      <c r="L43" s="143" t="s">
         <v>38</v>
       </c>
-      <c r="M43" s="87"/>
-      <c r="N43" s="79" t="s">
+      <c r="M43" s="144"/>
+      <c r="N43" s="136" t="s">
         <v>32</v>
       </c>
-      <c r="O43" s="80"/>
-      <c r="P43" s="81"/>
-      <c r="Q43" s="75"/>
-      <c r="R43" s="76"/>
-      <c r="S43" s="77"/>
-      <c r="T43" s="75"/>
-      <c r="U43" s="76"/>
-      <c r="V43" s="77"/>
-      <c r="W43" s="75"/>
-      <c r="X43" s="76"/>
-      <c r="Y43" s="77"/>
-      <c r="Z43" s="91" t="s">
+      <c r="O43" s="137"/>
+      <c r="P43" s="138"/>
+      <c r="Q43" s="129"/>
+      <c r="R43" s="130"/>
+      <c r="S43" s="131"/>
+      <c r="T43" s="129"/>
+      <c r="U43" s="130"/>
+      <c r="V43" s="131"/>
+      <c r="W43" s="129"/>
+      <c r="X43" s="130"/>
+      <c r="Y43" s="131"/>
+      <c r="Z43" s="123" t="s">
         <v>31</v>
       </c>
-      <c r="AA43" s="92"/>
-      <c r="AB43" s="92"/>
-      <c r="AC43" s="93"/>
-      <c r="AD43" s="75"/>
-      <c r="AE43" s="76"/>
-      <c r="AF43" s="77"/>
-      <c r="AG43" s="75"/>
-      <c r="AH43" s="76"/>
-      <c r="AI43" s="77"/>
-      <c r="AJ43" s="75"/>
-      <c r="AK43" s="76"/>
-      <c r="AL43" s="77"/>
-      <c r="AM43" s="75"/>
-      <c r="AN43" s="76"/>
-      <c r="AO43" s="77"/>
-      <c r="AP43" s="75"/>
-      <c r="AQ43" s="76"/>
-      <c r="AR43" s="77"/>
-      <c r="AS43" s="97" t="s">
+      <c r="AA43" s="124"/>
+      <c r="AB43" s="124"/>
+      <c r="AC43" s="125"/>
+      <c r="AD43" s="129"/>
+      <c r="AE43" s="130"/>
+      <c r="AF43" s="131"/>
+      <c r="AG43" s="129"/>
+      <c r="AH43" s="130"/>
+      <c r="AI43" s="131"/>
+      <c r="AJ43" s="129"/>
+      <c r="AK43" s="130"/>
+      <c r="AL43" s="131"/>
+      <c r="AM43" s="129"/>
+      <c r="AN43" s="130"/>
+      <c r="AO43" s="131"/>
+      <c r="AP43" s="129"/>
+      <c r="AQ43" s="130"/>
+      <c r="AR43" s="131"/>
+      <c r="AS43" s="132" t="s">
         <v>30</v>
       </c>
-      <c r="AT43" s="97"/>
-      <c r="AU43" s="97"/>
-      <c r="AV43" s="97"/>
-      <c r="AW43" s="75"/>
-      <c r="AX43" s="76"/>
-      <c r="AY43" s="77"/>
-      <c r="AZ43" s="75"/>
-      <c r="BA43" s="76"/>
-      <c r="BB43" s="77"/>
-      <c r="BC43" s="75"/>
-      <c r="BD43" s="76"/>
-      <c r="BE43" s="77"/>
-      <c r="BF43" s="75"/>
-      <c r="BG43" s="76"/>
-      <c r="BH43" s="77"/>
-      <c r="BI43" s="75"/>
-      <c r="BJ43" s="76"/>
-      <c r="BK43" s="77"/>
-      <c r="BL43" s="75"/>
-      <c r="BM43" s="76"/>
-      <c r="BN43" s="77"/>
-      <c r="BO43" s="75"/>
-      <c r="BP43" s="76"/>
-      <c r="BQ43" s="77"/>
-      <c r="BR43" s="75"/>
-      <c r="BS43" s="76"/>
-      <c r="BT43" s="77"/>
-    </row>
-    <row r="44" spans="1:72" x14ac:dyDescent="0.35">
-      <c r="A44" s="88" t="s">
+      <c r="AT43" s="132"/>
+      <c r="AU43" s="132"/>
+      <c r="AV43" s="132"/>
+      <c r="AW43" s="129"/>
+      <c r="AX43" s="130"/>
+      <c r="AY43" s="131"/>
+      <c r="AZ43" s="129"/>
+      <c r="BA43" s="130"/>
+      <c r="BB43" s="131"/>
+      <c r="BC43" s="129"/>
+      <c r="BD43" s="130"/>
+      <c r="BE43" s="131"/>
+      <c r="BF43" s="129"/>
+      <c r="BG43" s="130"/>
+      <c r="BH43" s="131"/>
+      <c r="BI43" s="129"/>
+      <c r="BJ43" s="130"/>
+      <c r="BK43" s="131"/>
+      <c r="BL43" s="129"/>
+      <c r="BM43" s="130"/>
+      <c r="BN43" s="131"/>
+      <c r="BO43" s="129"/>
+      <c r="BP43" s="130"/>
+      <c r="BQ43" s="131"/>
+      <c r="BR43" s="129"/>
+      <c r="BS43" s="130"/>
+      <c r="BT43" s="131"/>
+    </row>
+    <row r="44" spans="1:72" x14ac:dyDescent="0.2">
+      <c r="A44" s="120" t="s">
         <v>33</v>
       </c>
-      <c r="B44" s="89"/>
-      <c r="C44" s="63" t="s">
+      <c r="B44" s="121"/>
+      <c r="C44" s="119" t="s">
         <v>29</v>
       </c>
-      <c r="D44" s="63"/>
-      <c r="E44" s="63"/>
-      <c r="F44" s="63"/>
-      <c r="G44" s="78"/>
-      <c r="H44" s="78"/>
-      <c r="I44" s="78"/>
-      <c r="J44" s="78"/>
-      <c r="K44" s="78"/>
-      <c r="L44" s="85"/>
-      <c r="M44" s="85"/>
-      <c r="N44" s="82"/>
-      <c r="O44" s="83"/>
-      <c r="P44" s="84"/>
-      <c r="Q44" s="63" t="s">
+      <c r="D44" s="119"/>
+      <c r="E44" s="119"/>
+      <c r="F44" s="119"/>
+      <c r="G44" s="135"/>
+      <c r="H44" s="135"/>
+      <c r="I44" s="135"/>
+      <c r="J44" s="135"/>
+      <c r="K44" s="135"/>
+      <c r="L44" s="142"/>
+      <c r="M44" s="142"/>
+      <c r="N44" s="139"/>
+      <c r="O44" s="140"/>
+      <c r="P44" s="141"/>
+      <c r="Q44" s="119" t="s">
         <v>29</v>
       </c>
-      <c r="R44" s="63"/>
-      <c r="S44" s="63"/>
-      <c r="T44" s="63" t="s">
+      <c r="R44" s="119"/>
+      <c r="S44" s="119"/>
+      <c r="T44" s="119" t="s">
         <v>29</v>
       </c>
-      <c r="U44" s="63"/>
-      <c r="V44" s="63"/>
-      <c r="W44" s="63" t="s">
+      <c r="U44" s="119"/>
+      <c r="V44" s="119"/>
+      <c r="W44" s="119" t="s">
         <v>29</v>
       </c>
-      <c r="X44" s="63"/>
-      <c r="Y44" s="63"/>
-      <c r="Z44" s="94"/>
-      <c r="AA44" s="95"/>
-      <c r="AB44" s="95"/>
-      <c r="AC44" s="96"/>
-      <c r="AD44" s="63" t="s">
+      <c r="X44" s="119"/>
+      <c r="Y44" s="119"/>
+      <c r="Z44" s="126"/>
+      <c r="AA44" s="127"/>
+      <c r="AB44" s="127"/>
+      <c r="AC44" s="128"/>
+      <c r="AD44" s="119" t="s">
         <v>29</v>
       </c>
-      <c r="AE44" s="63"/>
-      <c r="AF44" s="63"/>
-      <c r="AG44" s="63" t="s">
+      <c r="AE44" s="119"/>
+      <c r="AF44" s="119"/>
+      <c r="AG44" s="119" t="s">
         <v>29</v>
       </c>
-      <c r="AH44" s="63"/>
-      <c r="AI44" s="63"/>
-      <c r="AJ44" s="63" t="s">
+      <c r="AH44" s="119"/>
+      <c r="AI44" s="119"/>
+      <c r="AJ44" s="119" t="s">
         <v>29</v>
       </c>
-      <c r="AK44" s="63"/>
-      <c r="AL44" s="63"/>
-      <c r="AM44" s="63" t="s">
+      <c r="AK44" s="119"/>
+      <c r="AL44" s="119"/>
+      <c r="AM44" s="119" t="s">
         <v>29</v>
       </c>
-      <c r="AN44" s="63"/>
-      <c r="AO44" s="63"/>
-      <c r="AP44" s="63" t="s">
+      <c r="AN44" s="119"/>
+      <c r="AO44" s="119"/>
+      <c r="AP44" s="119" t="s">
         <v>29</v>
       </c>
-      <c r="AQ44" s="63"/>
-      <c r="AR44" s="63"/>
-      <c r="AS44" s="97"/>
-      <c r="AT44" s="97"/>
-      <c r="AU44" s="97"/>
-      <c r="AV44" s="97"/>
-      <c r="AW44" s="63" t="s">
+      <c r="AQ44" s="119"/>
+      <c r="AR44" s="119"/>
+      <c r="AS44" s="132"/>
+      <c r="AT44" s="132"/>
+      <c r="AU44" s="132"/>
+      <c r="AV44" s="132"/>
+      <c r="AW44" s="119" t="s">
         <v>29</v>
       </c>
-      <c r="AX44" s="63"/>
-      <c r="AY44" s="63"/>
-      <c r="AZ44" s="63" t="s">
+      <c r="AX44" s="119"/>
+      <c r="AY44" s="119"/>
+      <c r="AZ44" s="119" t="s">
         <v>29</v>
       </c>
-      <c r="BA44" s="63"/>
-      <c r="BB44" s="63"/>
-      <c r="BC44" s="63" t="s">
+      <c r="BA44" s="119"/>
+      <c r="BB44" s="119"/>
+      <c r="BC44" s="119" t="s">
         <v>29</v>
       </c>
-      <c r="BD44" s="63"/>
-      <c r="BE44" s="63"/>
-      <c r="BF44" s="63" t="s">
+      <c r="BD44" s="119"/>
+      <c r="BE44" s="119"/>
+      <c r="BF44" s="119" t="s">
         <v>29</v>
       </c>
-      <c r="BG44" s="63"/>
-      <c r="BH44" s="63"/>
-      <c r="BI44" s="63" t="s">
+      <c r="BG44" s="119"/>
+      <c r="BH44" s="119"/>
+      <c r="BI44" s="119" t="s">
         <v>29</v>
       </c>
-      <c r="BJ44" s="63"/>
-      <c r="BK44" s="63"/>
-      <c r="BL44" s="63" t="s">
+      <c r="BJ44" s="119"/>
+      <c r="BK44" s="119"/>
+      <c r="BL44" s="119" t="s">
         <v>29</v>
       </c>
-      <c r="BM44" s="63"/>
-      <c r="BN44" s="63"/>
-      <c r="BO44" s="63" t="s">
+      <c r="BM44" s="119"/>
+      <c r="BN44" s="119"/>
+      <c r="BO44" s="119" t="s">
         <v>29</v>
       </c>
-      <c r="BP44" s="63"/>
-      <c r="BQ44" s="63"/>
-      <c r="BR44" s="63" t="s">
+      <c r="BP44" s="119"/>
+      <c r="BQ44" s="119"/>
+      <c r="BR44" s="119" t="s">
         <v>29</v>
       </c>
-      <c r="BS44" s="63"/>
-      <c r="BT44" s="63"/>
-    </row>
-    <row r="45" spans="1:72" x14ac:dyDescent="0.35">
-      <c r="A45" s="61" t="s">
+      <c r="BS44" s="119"/>
+      <c r="BT44" s="119"/>
+    </row>
+    <row r="45" spans="1:72" x14ac:dyDescent="0.2">
+      <c r="A45" s="133" t="s">
         <v>42</v>
       </c>
-      <c r="B45" s="62"/>
-      <c r="C45" s="142" t="s">
+      <c r="B45" s="134"/>
+      <c r="C45" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="D45" s="143"/>
-      <c r="E45" s="143"/>
-      <c r="F45" s="144"/>
-      <c r="G45" s="142" t="s">
+      <c r="D45" s="62"/>
+      <c r="E45" s="62"/>
+      <c r="F45" s="63"/>
+      <c r="G45" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="H45" s="143"/>
-      <c r="I45" s="144"/>
-      <c r="J45" s="142" t="s">
+      <c r="H45" s="62"/>
+      <c r="I45" s="63"/>
+      <c r="J45" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="K45" s="143"/>
-      <c r="L45" s="144"/>
-      <c r="M45" s="142" t="s">
+      <c r="K45" s="62"/>
+      <c r="L45" s="63"/>
+      <c r="M45" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="N45" s="143"/>
-      <c r="O45" s="144"/>
-      <c r="P45" s="142" t="s">
+      <c r="N45" s="62"/>
+      <c r="O45" s="63"/>
+      <c r="P45" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="Q45" s="143"/>
-      <c r="R45" s="144"/>
-      <c r="S45" s="142" t="s">
+      <c r="Q45" s="62"/>
+      <c r="R45" s="63"/>
+      <c r="S45" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="T45" s="143"/>
-      <c r="U45" s="144"/>
-      <c r="V45" s="142" t="s">
+      <c r="T45" s="62"/>
+      <c r="U45" s="63"/>
+      <c r="V45" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="W45" s="143"/>
-      <c r="X45" s="144"/>
-      <c r="Y45" s="142" t="s">
+      <c r="W45" s="62"/>
+      <c r="X45" s="63"/>
+      <c r="Y45" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="Z45" s="143"/>
-      <c r="AA45" s="144"/>
-      <c r="AB45" s="142" t="s">
+      <c r="Z45" s="62"/>
+      <c r="AA45" s="63"/>
+      <c r="AB45" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="AC45" s="143"/>
-      <c r="AD45" s="144"/>
-      <c r="AE45" s="142" t="s">
+      <c r="AC45" s="62"/>
+      <c r="AD45" s="63"/>
+      <c r="AE45" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="AF45" s="143"/>
-      <c r="AG45" s="144"/>
-      <c r="AH45" s="142" t="s">
+      <c r="AF45" s="62"/>
+      <c r="AG45" s="63"/>
+      <c r="AH45" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="AI45" s="143"/>
-      <c r="AJ45" s="144"/>
-      <c r="AK45" s="142" t="s">
+      <c r="AI45" s="62"/>
+      <c r="AJ45" s="63"/>
+      <c r="AK45" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="AL45" s="143"/>
-      <c r="AM45" s="144"/>
-      <c r="AN45" s="142" t="s">
+      <c r="AL45" s="62"/>
+      <c r="AM45" s="63"/>
+      <c r="AN45" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="AO45" s="143"/>
-      <c r="AP45" s="144"/>
-      <c r="AQ45" s="142" t="s">
+      <c r="AO45" s="62"/>
+      <c r="AP45" s="63"/>
+      <c r="AQ45" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="AR45" s="143"/>
-      <c r="AS45" s="144"/>
-      <c r="AT45" s="142" t="s">
+      <c r="AR45" s="62"/>
+      <c r="AS45" s="63"/>
+      <c r="AT45" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="AU45" s="143"/>
-      <c r="AV45" s="144"/>
-      <c r="AW45" s="142" t="s">
+      <c r="AU45" s="62"/>
+      <c r="AV45" s="63"/>
+      <c r="AW45" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="AX45" s="143"/>
-      <c r="AY45" s="144"/>
-      <c r="AZ45" s="142" t="s">
+      <c r="AX45" s="62"/>
+      <c r="AY45" s="63"/>
+      <c r="AZ45" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="BA45" s="143"/>
-      <c r="BB45" s="144"/>
-      <c r="BC45" s="142" t="s">
+      <c r="BA45" s="62"/>
+      <c r="BB45" s="63"/>
+      <c r="BC45" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="BD45" s="143"/>
-      <c r="BE45" s="144"/>
-      <c r="BF45" s="142" t="s">
+      <c r="BD45" s="62"/>
+      <c r="BE45" s="63"/>
+      <c r="BF45" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="BG45" s="143"/>
-      <c r="BH45" s="144"/>
-      <c r="BI45" s="142" t="s">
+      <c r="BG45" s="62"/>
+      <c r="BH45" s="63"/>
+      <c r="BI45" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="BJ45" s="143"/>
-      <c r="BK45" s="144"/>
-      <c r="BL45" s="142" t="s">
+      <c r="BJ45" s="62"/>
+      <c r="BK45" s="63"/>
+      <c r="BL45" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="BM45" s="143"/>
-      <c r="BN45" s="144"/>
-      <c r="BO45" s="142" t="s">
+      <c r="BM45" s="62"/>
+      <c r="BN45" s="63"/>
+      <c r="BO45" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="BP45" s="143"/>
-      <c r="BQ45" s="144"/>
-      <c r="BR45" s="142" t="s">
+      <c r="BP45" s="62"/>
+      <c r="BQ45" s="63"/>
+      <c r="BR45" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="BS45" s="143"/>
-      <c r="BT45" s="144"/>
+      <c r="BS45" s="62"/>
+      <c r="BT45" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="111">
-    <mergeCell ref="BL45:BN45"/>
-    <mergeCell ref="BO45:BQ45"/>
-    <mergeCell ref="BR45:BT45"/>
-    <mergeCell ref="C45:F45"/>
-    <mergeCell ref="G45:I45"/>
-    <mergeCell ref="J45:L45"/>
-    <mergeCell ref="M45:O45"/>
-    <mergeCell ref="P45:R45"/>
-    <mergeCell ref="S45:U45"/>
-    <mergeCell ref="V45:X45"/>
-    <mergeCell ref="Y45:AA45"/>
-    <mergeCell ref="AB45:AD45"/>
-    <mergeCell ref="AE45:AG45"/>
-    <mergeCell ref="AH45:AJ45"/>
-    <mergeCell ref="AK45:AM45"/>
-    <mergeCell ref="AN45:AP45"/>
-    <mergeCell ref="AZ45:BB45"/>
-    <mergeCell ref="BC45:BE45"/>
-    <mergeCell ref="BF45:BH45"/>
-    <mergeCell ref="BI45:BK45"/>
-    <mergeCell ref="AQ45:AS45"/>
-    <mergeCell ref="AT45:AV45"/>
-    <mergeCell ref="AW45:AY45"/>
-    <mergeCell ref="E39:H39"/>
-    <mergeCell ref="E40:H42"/>
-    <mergeCell ref="U25:AF25"/>
-    <mergeCell ref="U24:AF24"/>
-    <mergeCell ref="U23:AF23"/>
-    <mergeCell ref="AG23:BA23"/>
-    <mergeCell ref="AG24:BA24"/>
-    <mergeCell ref="AG25:BA25"/>
-    <mergeCell ref="U29:AF29"/>
-    <mergeCell ref="U28:AF28"/>
-    <mergeCell ref="U27:AF27"/>
-    <mergeCell ref="U26:AF26"/>
-    <mergeCell ref="AG26:BA26"/>
-    <mergeCell ref="AG27:BA27"/>
-    <mergeCell ref="AG28:BA28"/>
-    <mergeCell ref="AG29:BA29"/>
-    <mergeCell ref="P40:S42"/>
-    <mergeCell ref="X39:AC39"/>
-    <mergeCell ref="X40:AC42"/>
-    <mergeCell ref="BL39:BT39"/>
-    <mergeCell ref="BL40:BT42"/>
-    <mergeCell ref="BJ40:BK42"/>
-    <mergeCell ref="BE40:BI42"/>
-    <mergeCell ref="AZ40:BD42"/>
-    <mergeCell ref="AU40:AY42"/>
-    <mergeCell ref="BJ39:BK39"/>
-    <mergeCell ref="AO40:AT42"/>
-    <mergeCell ref="AD39:AK39"/>
-    <mergeCell ref="AD40:AK42"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="AG44:AI44"/>
+    <mergeCell ref="AO39:AT39"/>
+    <mergeCell ref="I39:M39"/>
+    <mergeCell ref="I40:M42"/>
+    <mergeCell ref="N39:O39"/>
+    <mergeCell ref="N40:O42"/>
+    <mergeCell ref="T43:V43"/>
+    <mergeCell ref="W43:Y43"/>
+    <mergeCell ref="AG43:AI43"/>
+    <mergeCell ref="AJ43:AL43"/>
+    <mergeCell ref="AM43:AO43"/>
+    <mergeCell ref="AP43:AR43"/>
+    <mergeCell ref="C44:F44"/>
+    <mergeCell ref="G44:K44"/>
+    <mergeCell ref="N43:P44"/>
+    <mergeCell ref="L44:M44"/>
+    <mergeCell ref="L43:M43"/>
+    <mergeCell ref="AD44:AF44"/>
+    <mergeCell ref="AD43:AF43"/>
+    <mergeCell ref="Q43:S43"/>
+    <mergeCell ref="A40:D42"/>
+    <mergeCell ref="P39:S39"/>
+    <mergeCell ref="A39:D39"/>
+    <mergeCell ref="BR43:BT43"/>
+    <mergeCell ref="BF43:BH43"/>
+    <mergeCell ref="BI43:BK43"/>
+    <mergeCell ref="BL43:BN43"/>
+    <mergeCell ref="BO43:BQ43"/>
+    <mergeCell ref="BC44:BE44"/>
+    <mergeCell ref="BF44:BH44"/>
+    <mergeCell ref="BI44:BK44"/>
+    <mergeCell ref="BL44:BN44"/>
+    <mergeCell ref="BR44:BT44"/>
+    <mergeCell ref="BO44:BQ44"/>
     <mergeCell ref="AW44:AY44"/>
     <mergeCell ref="AZ44:BB44"/>
     <mergeCell ref="AM44:AO44"/>
@@ -5456,41 +5439,58 @@
     <mergeCell ref="AW43:AY43"/>
     <mergeCell ref="AZ43:BB43"/>
     <mergeCell ref="C43:F43"/>
-    <mergeCell ref="BR43:BT43"/>
-    <mergeCell ref="BF43:BH43"/>
-    <mergeCell ref="BI43:BK43"/>
-    <mergeCell ref="BL43:BN43"/>
-    <mergeCell ref="BO43:BQ43"/>
-    <mergeCell ref="BC44:BE44"/>
-    <mergeCell ref="BF44:BH44"/>
-    <mergeCell ref="BI44:BK44"/>
-    <mergeCell ref="BL44:BN44"/>
-    <mergeCell ref="BR44:BT44"/>
-    <mergeCell ref="BO44:BQ44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="AG44:AI44"/>
-    <mergeCell ref="AO39:AT39"/>
-    <mergeCell ref="I39:M39"/>
-    <mergeCell ref="I40:M42"/>
-    <mergeCell ref="N39:O39"/>
-    <mergeCell ref="N40:O42"/>
-    <mergeCell ref="T43:V43"/>
-    <mergeCell ref="W43:Y43"/>
-    <mergeCell ref="AG43:AI43"/>
-    <mergeCell ref="AJ43:AL43"/>
-    <mergeCell ref="AM43:AO43"/>
-    <mergeCell ref="AP43:AR43"/>
-    <mergeCell ref="C44:F44"/>
-    <mergeCell ref="G44:K44"/>
-    <mergeCell ref="N43:P44"/>
-    <mergeCell ref="L44:M44"/>
-    <mergeCell ref="L43:M43"/>
-    <mergeCell ref="AD44:AF44"/>
-    <mergeCell ref="AD43:AF43"/>
-    <mergeCell ref="Q43:S43"/>
-    <mergeCell ref="A40:D42"/>
-    <mergeCell ref="P39:S39"/>
-    <mergeCell ref="A39:D39"/>
+    <mergeCell ref="BL39:BT39"/>
+    <mergeCell ref="BL40:BT42"/>
+    <mergeCell ref="BJ40:BK42"/>
+    <mergeCell ref="BE40:BI42"/>
+    <mergeCell ref="AZ40:BD42"/>
+    <mergeCell ref="AU40:AY42"/>
+    <mergeCell ref="BJ39:BK39"/>
+    <mergeCell ref="AO40:AT42"/>
+    <mergeCell ref="AD39:AK39"/>
+    <mergeCell ref="AD40:AK42"/>
+    <mergeCell ref="E39:H39"/>
+    <mergeCell ref="E40:H42"/>
+    <mergeCell ref="U25:AF25"/>
+    <mergeCell ref="U24:AF24"/>
+    <mergeCell ref="U23:AF23"/>
+    <mergeCell ref="AG23:BA23"/>
+    <mergeCell ref="AG24:BA24"/>
+    <mergeCell ref="AG25:BA25"/>
+    <mergeCell ref="U29:AF29"/>
+    <mergeCell ref="U28:AF28"/>
+    <mergeCell ref="U27:AF27"/>
+    <mergeCell ref="U26:AF26"/>
+    <mergeCell ref="AG26:BA26"/>
+    <mergeCell ref="AG27:BA27"/>
+    <mergeCell ref="AG28:BA28"/>
+    <mergeCell ref="AG29:BA29"/>
+    <mergeCell ref="P40:S42"/>
+    <mergeCell ref="X39:AC39"/>
+    <mergeCell ref="X40:AC42"/>
+    <mergeCell ref="BL45:BN45"/>
+    <mergeCell ref="BO45:BQ45"/>
+    <mergeCell ref="BR45:BT45"/>
+    <mergeCell ref="C45:F45"/>
+    <mergeCell ref="G45:I45"/>
+    <mergeCell ref="J45:L45"/>
+    <mergeCell ref="M45:O45"/>
+    <mergeCell ref="P45:R45"/>
+    <mergeCell ref="S45:U45"/>
+    <mergeCell ref="V45:X45"/>
+    <mergeCell ref="Y45:AA45"/>
+    <mergeCell ref="AB45:AD45"/>
+    <mergeCell ref="AE45:AG45"/>
+    <mergeCell ref="AH45:AJ45"/>
+    <mergeCell ref="AK45:AM45"/>
+    <mergeCell ref="AN45:AP45"/>
+    <mergeCell ref="AZ45:BB45"/>
+    <mergeCell ref="BC45:BE45"/>
+    <mergeCell ref="BF45:BH45"/>
+    <mergeCell ref="BI45:BK45"/>
+    <mergeCell ref="AQ45:AS45"/>
+    <mergeCell ref="AT45:AV45"/>
+    <mergeCell ref="AW45:AY45"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="99" fitToHeight="0" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>